<commit_message>
Testcases Added in Documentation
</commit_message>
<xml_diff>
--- a/Docs/M120_ZeitPlan.xlsx
+++ b/Docs/M120_ZeitPlan.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D1DB27B-1CAC-4729-BD8F-251081FD49B4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>IPERKA</t>
   </si>
@@ -118,7 +117,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -733,7 +732,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="188">
+  <cellXfs count="194">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -893,127 +892,15 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1021,27 +908,145 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1321,29 +1326,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="T30" sqref="T30:V30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42" bestFit="1" customWidth="1"/>
-    <col min="3" max="42" width="5.6640625" customWidth="1"/>
+    <col min="3" max="42" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="179" t="s">
+    <row r="1" spans="1:38" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="181" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="180"/>
-      <c r="C1" s="180"/>
-      <c r="D1" s="180"/>
-      <c r="E1" s="180"/>
-      <c r="F1" s="180"/>
+      <c r="B1" s="182"/>
+      <c r="C1" s="182"/>
+      <c r="D1" s="182"/>
+      <c r="E1" s="182"/>
+      <c r="F1" s="182"/>
       <c r="G1" s="74"/>
       <c r="H1" s="74"/>
       <c r="I1" s="74"/>
@@ -1360,30 +1365,30 @@
       <c r="T1" s="74"/>
       <c r="U1" s="74"/>
       <c r="V1" s="75"/>
-      <c r="W1" s="170"/>
-      <c r="X1" s="170"/>
-      <c r="Y1" s="170"/>
-      <c r="Z1" s="170"/>
-      <c r="AA1" s="170"/>
-      <c r="AB1" s="170"/>
-      <c r="AC1" s="170"/>
-      <c r="AD1" s="170"/>
-      <c r="AE1" s="170"/>
-      <c r="AF1" s="170"/>
-      <c r="AG1" s="170"/>
-      <c r="AH1" s="170"/>
-      <c r="AI1" s="170"/>
-      <c r="AJ1" s="170"/>
-      <c r="AK1" s="170"/>
-      <c r="AL1" s="170"/>
-    </row>
-    <row r="2" spans="1:38" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="181"/>
-      <c r="B2" s="182"/>
-      <c r="C2" s="182"/>
-      <c r="D2" s="182"/>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
+      <c r="W1" s="134"/>
+      <c r="X1" s="134"/>
+      <c r="Y1" s="134"/>
+      <c r="Z1" s="134"/>
+      <c r="AA1" s="134"/>
+      <c r="AB1" s="134"/>
+      <c r="AC1" s="134"/>
+      <c r="AD1" s="134"/>
+      <c r="AE1" s="134"/>
+      <c r="AF1" s="134"/>
+      <c r="AG1" s="134"/>
+      <c r="AH1" s="134"/>
+      <c r="AI1" s="134"/>
+      <c r="AJ1" s="134"/>
+      <c r="AK1" s="134"/>
+      <c r="AL1" s="134"/>
+    </row>
+    <row r="2" spans="1:38" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="183"/>
+      <c r="B2" s="184"/>
+      <c r="C2" s="184"/>
+      <c r="D2" s="184"/>
+      <c r="E2" s="184"/>
+      <c r="F2" s="184"/>
       <c r="G2" s="79"/>
       <c r="H2" s="81" t="s">
         <v>10</v>
@@ -1397,37 +1402,37 @@
       </c>
       <c r="N2" s="82"/>
       <c r="O2" s="83"/>
-      <c r="P2" s="173"/>
-      <c r="Q2" s="173"/>
-      <c r="R2" s="173"/>
-      <c r="S2" s="173"/>
-      <c r="T2" s="173"/>
-      <c r="U2" s="173"/>
+      <c r="P2" s="136"/>
+      <c r="Q2" s="136"/>
+      <c r="R2" s="136"/>
+      <c r="S2" s="136"/>
+      <c r="T2" s="136"/>
+      <c r="U2" s="136"/>
       <c r="V2" s="76"/>
-      <c r="W2" s="170"/>
-      <c r="X2" s="170"/>
-      <c r="Y2" s="170"/>
-      <c r="Z2" s="170"/>
-      <c r="AA2" s="170"/>
-      <c r="AB2" s="170"/>
-      <c r="AC2" s="170"/>
-      <c r="AD2" s="170"/>
-      <c r="AE2" s="170"/>
-      <c r="AF2" s="170"/>
-      <c r="AG2" s="170"/>
-      <c r="AH2" s="170"/>
-      <c r="AI2" s="170"/>
-      <c r="AJ2" s="170"/>
-      <c r="AK2" s="170"/>
-      <c r="AL2" s="170"/>
-    </row>
-    <row r="3" spans="1:38" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="181"/>
-      <c r="B3" s="182"/>
-      <c r="C3" s="182"/>
-      <c r="D3" s="182"/>
-      <c r="E3" s="182"/>
-      <c r="F3" s="182"/>
+      <c r="W2" s="134"/>
+      <c r="X2" s="134"/>
+      <c r="Y2" s="134"/>
+      <c r="Z2" s="134"/>
+      <c r="AA2" s="134"/>
+      <c r="AB2" s="134"/>
+      <c r="AC2" s="134"/>
+      <c r="AD2" s="134"/>
+      <c r="AE2" s="134"/>
+      <c r="AF2" s="134"/>
+      <c r="AG2" s="134"/>
+      <c r="AH2" s="134"/>
+      <c r="AI2" s="134"/>
+      <c r="AJ2" s="134"/>
+      <c r="AK2" s="134"/>
+      <c r="AL2" s="134"/>
+    </row>
+    <row r="3" spans="1:38" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="183"/>
+      <c r="B3" s="184"/>
+      <c r="C3" s="184"/>
+      <c r="D3" s="184"/>
+      <c r="E3" s="184"/>
+      <c r="F3" s="184"/>
       <c r="G3" s="80"/>
       <c r="H3" s="81" t="s">
         <v>11</v>
@@ -1441,37 +1446,37 @@
       </c>
       <c r="N3" s="77"/>
       <c r="O3" s="78"/>
-      <c r="P3" s="173"/>
-      <c r="Q3" s="173"/>
-      <c r="R3" s="173"/>
-      <c r="S3" s="173"/>
-      <c r="T3" s="173"/>
-      <c r="U3" s="173"/>
+      <c r="P3" s="136"/>
+      <c r="Q3" s="136"/>
+      <c r="R3" s="136"/>
+      <c r="S3" s="136"/>
+      <c r="T3" s="136"/>
+      <c r="U3" s="136"/>
       <c r="V3" s="76"/>
-      <c r="W3" s="170"/>
-      <c r="X3" s="170"/>
-      <c r="Y3" s="170"/>
-      <c r="Z3" s="170"/>
-      <c r="AA3" s="170"/>
-      <c r="AB3" s="170"/>
-      <c r="AC3" s="170"/>
-      <c r="AD3" s="170"/>
-      <c r="AE3" s="170"/>
-      <c r="AF3" s="170"/>
-      <c r="AG3" s="170"/>
-      <c r="AH3" s="170"/>
-      <c r="AI3" s="170"/>
-      <c r="AJ3" s="170"/>
-      <c r="AK3" s="170"/>
-      <c r="AL3" s="170"/>
-    </row>
-    <row r="4" spans="1:38" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="183"/>
-      <c r="B4" s="184"/>
-      <c r="C4" s="184"/>
-      <c r="D4" s="184"/>
-      <c r="E4" s="184"/>
-      <c r="F4" s="184"/>
+      <c r="W3" s="134"/>
+      <c r="X3" s="134"/>
+      <c r="Y3" s="134"/>
+      <c r="Z3" s="134"/>
+      <c r="AA3" s="134"/>
+      <c r="AB3" s="134"/>
+      <c r="AC3" s="134"/>
+      <c r="AD3" s="134"/>
+      <c r="AE3" s="134"/>
+      <c r="AF3" s="134"/>
+      <c r="AG3" s="134"/>
+      <c r="AH3" s="134"/>
+      <c r="AI3" s="134"/>
+      <c r="AJ3" s="134"/>
+      <c r="AK3" s="134"/>
+      <c r="AL3" s="134"/>
+    </row>
+    <row r="4" spans="1:38" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="185"/>
+      <c r="B4" s="186"/>
+      <c r="C4" s="186"/>
+      <c r="D4" s="186"/>
+      <c r="E4" s="186"/>
+      <c r="F4" s="186"/>
       <c r="G4" s="77"/>
       <c r="H4" s="77"/>
       <c r="I4" s="77"/>
@@ -1488,138 +1493,138 @@
       <c r="T4" s="77"/>
       <c r="U4" s="77"/>
       <c r="V4" s="78"/>
-      <c r="W4" s="170"/>
-      <c r="X4" s="170"/>
-      <c r="Y4" s="170"/>
-      <c r="Z4" s="170"/>
-      <c r="AA4" s="170"/>
-      <c r="AB4" s="170"/>
-      <c r="AC4" s="170"/>
-      <c r="AD4" s="170"/>
-      <c r="AE4" s="170"/>
-      <c r="AF4" s="171"/>
-      <c r="AG4" s="171"/>
-      <c r="AH4" s="170"/>
-      <c r="AI4" s="170"/>
-      <c r="AJ4" s="171"/>
-      <c r="AK4" s="171"/>
-      <c r="AL4" s="171"/>
-    </row>
-    <row r="5" spans="1:38" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W4" s="134"/>
+      <c r="X4" s="134"/>
+      <c r="Y4" s="134"/>
+      <c r="Z4" s="134"/>
+      <c r="AA4" s="134"/>
+      <c r="AB4" s="134"/>
+      <c r="AC4" s="134"/>
+      <c r="AD4" s="134"/>
+      <c r="AE4" s="134"/>
+      <c r="AF4" s="135"/>
+      <c r="AG4" s="135"/>
+      <c r="AH4" s="134"/>
+      <c r="AI4" s="134"/>
+      <c r="AJ4" s="135"/>
+      <c r="AK4" s="135"/>
+      <c r="AL4" s="135"/>
+    </row>
+    <row r="5" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="136">
+      <c r="C5" s="178">
         <v>1</v>
       </c>
-      <c r="D5" s="135"/>
-      <c r="E5" s="135"/>
-      <c r="F5" s="137"/>
-      <c r="G5" s="135">
+      <c r="D5" s="179"/>
+      <c r="E5" s="179"/>
+      <c r="F5" s="180"/>
+      <c r="G5" s="179">
         <v>2</v>
       </c>
-      <c r="H5" s="135"/>
-      <c r="I5" s="135"/>
-      <c r="J5" s="135"/>
-      <c r="K5" s="136">
+      <c r="H5" s="179"/>
+      <c r="I5" s="179"/>
+      <c r="J5" s="179"/>
+      <c r="K5" s="178">
         <v>3</v>
       </c>
-      <c r="L5" s="135"/>
-      <c r="M5" s="135"/>
-      <c r="N5" s="137"/>
-      <c r="O5" s="135">
+      <c r="L5" s="179"/>
+      <c r="M5" s="179"/>
+      <c r="N5" s="180"/>
+      <c r="O5" s="179">
         <v>4</v>
       </c>
-      <c r="P5" s="135"/>
-      <c r="Q5" s="135"/>
-      <c r="R5" s="135"/>
-      <c r="S5" s="136">
+      <c r="P5" s="179"/>
+      <c r="Q5" s="179"/>
+      <c r="R5" s="179"/>
+      <c r="S5" s="178">
         <v>5</v>
       </c>
-      <c r="T5" s="135"/>
-      <c r="U5" s="135"/>
-      <c r="V5" s="137"/>
-      <c r="W5" s="172"/>
-      <c r="X5" s="172"/>
-      <c r="Y5" s="172"/>
-      <c r="Z5" s="172"/>
-      <c r="AA5" s="172"/>
-      <c r="AB5" s="172"/>
-      <c r="AC5" s="172"/>
-      <c r="AD5" s="172"/>
-      <c r="AE5" s="172"/>
-      <c r="AF5" s="172"/>
-      <c r="AG5" s="172"/>
-      <c r="AH5" s="172"/>
-      <c r="AI5" s="172"/>
-      <c r="AJ5" s="172"/>
-      <c r="AK5" s="172"/>
-      <c r="AL5" s="172"/>
-    </row>
-    <row r="6" spans="1:38" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="T5" s="179"/>
+      <c r="U5" s="179"/>
+      <c r="V5" s="180"/>
+      <c r="W5" s="144"/>
+      <c r="X5" s="144"/>
+      <c r="Y5" s="144"/>
+      <c r="Z5" s="144"/>
+      <c r="AA5" s="144"/>
+      <c r="AB5" s="144"/>
+      <c r="AC5" s="144"/>
+      <c r="AD5" s="144"/>
+      <c r="AE5" s="144"/>
+      <c r="AF5" s="144"/>
+      <c r="AG5" s="144"/>
+      <c r="AH5" s="144"/>
+      <c r="AI5" s="144"/>
+      <c r="AJ5" s="144"/>
+      <c r="AK5" s="144"/>
+      <c r="AL5" s="144"/>
+    </row>
+    <row r="6" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="138" t="s">
+      <c r="C6" s="165" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="139"/>
-      <c r="E6" s="139"/>
-      <c r="F6" s="140"/>
-      <c r="G6" s="138" t="s">
+      <c r="D6" s="166"/>
+      <c r="E6" s="166"/>
+      <c r="F6" s="167"/>
+      <c r="G6" s="165" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="139"/>
-      <c r="I6" s="139"/>
-      <c r="J6" s="140"/>
-      <c r="K6" s="138" t="s">
+      <c r="H6" s="166"/>
+      <c r="I6" s="166"/>
+      <c r="J6" s="167"/>
+      <c r="K6" s="165" t="s">
         <v>18</v>
       </c>
-      <c r="L6" s="139"/>
-      <c r="M6" s="139"/>
-      <c r="N6" s="140"/>
-      <c r="O6" s="138" t="s">
+      <c r="L6" s="166"/>
+      <c r="M6" s="166"/>
+      <c r="N6" s="167"/>
+      <c r="O6" s="165" t="s">
         <v>19</v>
       </c>
-      <c r="P6" s="139"/>
-      <c r="Q6" s="139"/>
-      <c r="R6" s="140"/>
-      <c r="S6" s="136" t="s">
+      <c r="P6" s="166"/>
+      <c r="Q6" s="166"/>
+      <c r="R6" s="167"/>
+      <c r="S6" s="178" t="s">
         <v>20</v>
       </c>
-      <c r="T6" s="135"/>
-      <c r="U6" s="135"/>
-      <c r="V6" s="137"/>
-      <c r="W6" s="172"/>
-      <c r="X6" s="172"/>
-      <c r="Y6" s="172"/>
-      <c r="Z6" s="172"/>
-      <c r="AA6" s="172"/>
-      <c r="AB6" s="172"/>
-      <c r="AC6" s="172"/>
-      <c r="AD6" s="172"/>
-      <c r="AE6" s="172"/>
-      <c r="AF6" s="172"/>
-      <c r="AG6" s="172"/>
-      <c r="AH6" s="172"/>
-      <c r="AI6" s="172"/>
-      <c r="AJ6" s="172"/>
-      <c r="AK6" s="172"/>
-      <c r="AL6" s="172"/>
-    </row>
-    <row r="7" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="166" t="s">
+      <c r="T6" s="179"/>
+      <c r="U6" s="179"/>
+      <c r="V6" s="180"/>
+      <c r="W6" s="144"/>
+      <c r="X6" s="144"/>
+      <c r="Y6" s="144"/>
+      <c r="Z6" s="144"/>
+      <c r="AA6" s="144"/>
+      <c r="AB6" s="144"/>
+      <c r="AC6" s="144"/>
+      <c r="AD6" s="144"/>
+      <c r="AE6" s="144"/>
+      <c r="AF6" s="144"/>
+      <c r="AG6" s="144"/>
+      <c r="AH6" s="144"/>
+      <c r="AI6" s="144"/>
+      <c r="AJ6" s="144"/>
+      <c r="AK6" s="144"/>
+      <c r="AL6" s="144"/>
+    </row>
+    <row r="7" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="161" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="168" t="s">
+      <c r="B7" s="163" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="176"/>
-      <c r="D7" s="175"/>
+      <c r="C7" s="138"/>
+      <c r="D7" s="137"/>
       <c r="E7" s="4"/>
       <c r="F7" s="5"/>
       <c r="G7" s="3"/>
@@ -1638,27 +1643,27 @@
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
       <c r="V7" s="5"/>
-      <c r="W7" s="171"/>
-      <c r="X7" s="171"/>
-      <c r="Y7" s="171"/>
-      <c r="Z7" s="171"/>
-      <c r="AA7" s="171"/>
-      <c r="AB7" s="171"/>
-      <c r="AC7" s="171"/>
-      <c r="AD7" s="171"/>
-      <c r="AE7" s="171"/>
-      <c r="AF7" s="171"/>
-      <c r="AG7" s="171"/>
-      <c r="AH7" s="171"/>
-      <c r="AI7" s="171"/>
-      <c r="AJ7" s="171"/>
-      <c r="AK7" s="171"/>
-      <c r="AL7" s="171"/>
-    </row>
-    <row r="8" spans="1:38" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="167"/>
-      <c r="B8" s="169"/>
-      <c r="C8" s="178"/>
+      <c r="W7" s="135"/>
+      <c r="X7" s="135"/>
+      <c r="Y7" s="135"/>
+      <c r="Z7" s="135"/>
+      <c r="AA7" s="135"/>
+      <c r="AB7" s="135"/>
+      <c r="AC7" s="135"/>
+      <c r="AD7" s="135"/>
+      <c r="AE7" s="135"/>
+      <c r="AF7" s="135"/>
+      <c r="AG7" s="135"/>
+      <c r="AH7" s="135"/>
+      <c r="AI7" s="135"/>
+      <c r="AJ7" s="135"/>
+      <c r="AK7" s="135"/>
+      <c r="AL7" s="135"/>
+    </row>
+    <row r="8" spans="1:38" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="162"/>
+      <c r="B8" s="164"/>
+      <c r="C8" s="140"/>
       <c r="D8" s="90"/>
       <c r="E8" s="86"/>
       <c r="F8" s="87"/>
@@ -1678,28 +1683,28 @@
       <c r="T8" s="86"/>
       <c r="U8" s="86"/>
       <c r="V8" s="87"/>
-      <c r="W8" s="171"/>
-      <c r="X8" s="171"/>
-      <c r="Y8" s="171"/>
-      <c r="Z8" s="171"/>
-      <c r="AA8" s="171"/>
-      <c r="AB8" s="171"/>
-      <c r="AC8" s="171"/>
-      <c r="AD8" s="171"/>
-      <c r="AE8" s="171"/>
-      <c r="AF8" s="171"/>
-      <c r="AG8" s="171"/>
-      <c r="AH8" s="171"/>
-      <c r="AI8" s="171"/>
-      <c r="AJ8" s="171"/>
-      <c r="AK8" s="171"/>
-      <c r="AL8" s="171"/>
-    </row>
-    <row r="9" spans="1:38" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="155" t="s">
+      <c r="W8" s="135"/>
+      <c r="X8" s="135"/>
+      <c r="Y8" s="135"/>
+      <c r="Z8" s="135"/>
+      <c r="AA8" s="135"/>
+      <c r="AB8" s="135"/>
+      <c r="AC8" s="135"/>
+      <c r="AD8" s="135"/>
+      <c r="AE8" s="135"/>
+      <c r="AF8" s="135"/>
+      <c r="AG8" s="135"/>
+      <c r="AH8" s="135"/>
+      <c r="AI8" s="135"/>
+      <c r="AJ8" s="135"/>
+      <c r="AK8" s="135"/>
+      <c r="AL8" s="135"/>
+    </row>
+    <row r="9" spans="1:38" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="150" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="158" t="s">
+      <c r="B9" s="153" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="19"/>
@@ -1722,31 +1727,31 @@
       <c r="T9" s="20"/>
       <c r="U9" s="20"/>
       <c r="V9" s="21"/>
-      <c r="W9" s="171"/>
-      <c r="X9" s="171"/>
-      <c r="Y9" s="171"/>
-      <c r="Z9" s="171"/>
-      <c r="AA9" s="171"/>
-      <c r="AB9" s="171"/>
-      <c r="AC9" s="171"/>
-      <c r="AD9" s="171"/>
-      <c r="AE9" s="171"/>
-      <c r="AF9" s="171"/>
-      <c r="AG9" s="171"/>
-      <c r="AH9" s="171"/>
-      <c r="AI9" s="171"/>
-      <c r="AJ9" s="171"/>
-      <c r="AK9" s="171"/>
-      <c r="AL9" s="171"/>
-    </row>
-    <row r="10" spans="1:38" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="156"/>
-      <c r="B10" s="159"/>
+      <c r="W9" s="135"/>
+      <c r="X9" s="135"/>
+      <c r="Y9" s="135"/>
+      <c r="Z9" s="135"/>
+      <c r="AA9" s="135"/>
+      <c r="AB9" s="135"/>
+      <c r="AC9" s="135"/>
+      <c r="AD9" s="135"/>
+      <c r="AE9" s="135"/>
+      <c r="AF9" s="135"/>
+      <c r="AG9" s="135"/>
+      <c r="AH9" s="135"/>
+      <c r="AI9" s="135"/>
+      <c r="AJ9" s="135"/>
+      <c r="AK9" s="135"/>
+      <c r="AL9" s="135"/>
+    </row>
+    <row r="10" spans="1:38" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="151"/>
+      <c r="B10" s="154"/>
       <c r="C10" s="92"/>
       <c r="D10" s="101"/>
       <c r="E10" s="101"/>
       <c r="F10" s="102"/>
-      <c r="G10" s="187"/>
+      <c r="G10" s="143"/>
       <c r="H10" s="99"/>
       <c r="I10" s="25"/>
       <c r="J10" s="26"/>
@@ -1762,32 +1767,32 @@
       <c r="T10" s="25"/>
       <c r="U10" s="25"/>
       <c r="V10" s="26"/>
-      <c r="W10" s="171"/>
-      <c r="X10" s="171"/>
-      <c r="Y10" s="171"/>
-      <c r="Z10" s="171"/>
-      <c r="AA10" s="171"/>
-      <c r="AB10" s="171"/>
-      <c r="AC10" s="171"/>
-      <c r="AD10" s="171"/>
-      <c r="AE10" s="171"/>
-      <c r="AF10" s="171"/>
-      <c r="AG10" s="171"/>
-      <c r="AH10" s="171"/>
-      <c r="AI10" s="171"/>
-      <c r="AJ10" s="171"/>
-      <c r="AK10" s="171"/>
-      <c r="AL10" s="171"/>
-    </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A11" s="156"/>
-      <c r="B11" s="160" t="s">
+      <c r="W10" s="135"/>
+      <c r="X10" s="135"/>
+      <c r="Y10" s="135"/>
+      <c r="Z10" s="135"/>
+      <c r="AA10" s="135"/>
+      <c r="AB10" s="135"/>
+      <c r="AC10" s="135"/>
+      <c r="AD10" s="135"/>
+      <c r="AE10" s="135"/>
+      <c r="AF10" s="135"/>
+      <c r="AG10" s="135"/>
+      <c r="AH10" s="135"/>
+      <c r="AI10" s="135"/>
+      <c r="AJ10" s="135"/>
+      <c r="AK10" s="135"/>
+      <c r="AL10" s="135"/>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A11" s="151"/>
+      <c r="B11" s="155" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
-      <c r="F11" s="177"/>
+      <c r="F11" s="139"/>
       <c r="G11" s="11"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
@@ -1804,26 +1809,26 @@
       <c r="T11" s="9"/>
       <c r="U11" s="9"/>
       <c r="V11" s="10"/>
-      <c r="W11" s="171"/>
-      <c r="X11" s="171"/>
-      <c r="Y11" s="171"/>
-      <c r="Z11" s="171"/>
-      <c r="AA11" s="171"/>
-      <c r="AB11" s="171"/>
-      <c r="AC11" s="171"/>
-      <c r="AD11" s="171"/>
-      <c r="AE11" s="171"/>
-      <c r="AF11" s="171"/>
-      <c r="AG11" s="171"/>
-      <c r="AH11" s="171"/>
-      <c r="AI11" s="171"/>
-      <c r="AJ11" s="171"/>
-      <c r="AK11" s="171"/>
-      <c r="AL11" s="171"/>
-    </row>
-    <row r="12" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="157"/>
-      <c r="B12" s="161"/>
+      <c r="W11" s="135"/>
+      <c r="X11" s="135"/>
+      <c r="Y11" s="135"/>
+      <c r="Z11" s="135"/>
+      <c r="AA11" s="135"/>
+      <c r="AB11" s="135"/>
+      <c r="AC11" s="135"/>
+      <c r="AD11" s="135"/>
+      <c r="AE11" s="135"/>
+      <c r="AF11" s="135"/>
+      <c r="AG11" s="135"/>
+      <c r="AH11" s="135"/>
+      <c r="AI11" s="135"/>
+      <c r="AJ11" s="135"/>
+      <c r="AK11" s="135"/>
+      <c r="AL11" s="135"/>
+    </row>
+    <row r="12" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="152"/>
+      <c r="B12" s="156"/>
       <c r="C12" s="18"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
@@ -1844,28 +1849,28 @@
       <c r="T12" s="14"/>
       <c r="U12" s="14"/>
       <c r="V12" s="15"/>
-      <c r="W12" s="171"/>
-      <c r="X12" s="171"/>
-      <c r="Y12" s="171"/>
-      <c r="Z12" s="171"/>
-      <c r="AA12" s="171"/>
-      <c r="AB12" s="171"/>
-      <c r="AC12" s="171"/>
-      <c r="AD12" s="171"/>
-      <c r="AE12" s="171"/>
-      <c r="AF12" s="171"/>
-      <c r="AG12" s="171"/>
-      <c r="AH12" s="171"/>
-      <c r="AI12" s="171"/>
-      <c r="AJ12" s="171"/>
-      <c r="AK12" s="171"/>
-      <c r="AL12" s="171"/>
-    </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A13" s="162" t="s">
+      <c r="W12" s="135"/>
+      <c r="X12" s="135"/>
+      <c r="Y12" s="135"/>
+      <c r="Z12" s="135"/>
+      <c r="AA12" s="135"/>
+      <c r="AB12" s="135"/>
+      <c r="AC12" s="135"/>
+      <c r="AD12" s="135"/>
+      <c r="AE12" s="135"/>
+      <c r="AF12" s="135"/>
+      <c r="AG12" s="135"/>
+      <c r="AH12" s="135"/>
+      <c r="AI12" s="135"/>
+      <c r="AJ12" s="135"/>
+      <c r="AK12" s="135"/>
+      <c r="AL12" s="135"/>
+    </row>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A13" s="157" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="164" t="s">
+      <c r="B13" s="159" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="30"/>
@@ -1888,33 +1893,33 @@
       <c r="T13" s="31"/>
       <c r="U13" s="31"/>
       <c r="V13" s="32"/>
-      <c r="W13" s="171"/>
-      <c r="X13" s="171"/>
-      <c r="Y13" s="171"/>
-      <c r="Z13" s="171"/>
-      <c r="AA13" s="171"/>
-      <c r="AB13" s="171"/>
-      <c r="AC13" s="171"/>
-      <c r="AD13" s="171"/>
-      <c r="AE13" s="171"/>
-      <c r="AF13" s="171"/>
-      <c r="AG13" s="171"/>
-      <c r="AH13" s="171"/>
-      <c r="AI13" s="171"/>
-      <c r="AJ13" s="171"/>
-      <c r="AK13" s="171"/>
-      <c r="AL13" s="171"/>
-    </row>
-    <row r="14" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="163"/>
-      <c r="B14" s="165"/>
+      <c r="W13" s="135"/>
+      <c r="X13" s="135"/>
+      <c r="Y13" s="135"/>
+      <c r="Z13" s="135"/>
+      <c r="AA13" s="135"/>
+      <c r="AB13" s="135"/>
+      <c r="AC13" s="135"/>
+      <c r="AD13" s="135"/>
+      <c r="AE13" s="135"/>
+      <c r="AF13" s="135"/>
+      <c r="AG13" s="135"/>
+      <c r="AH13" s="135"/>
+      <c r="AI13" s="135"/>
+      <c r="AJ13" s="135"/>
+      <c r="AK13" s="135"/>
+      <c r="AL13" s="135"/>
+    </row>
+    <row r="14" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="158"/>
+      <c r="B14" s="160"/>
       <c r="C14" s="35"/>
       <c r="D14" s="36"/>
       <c r="E14" s="36"/>
       <c r="F14" s="37"/>
       <c r="G14" s="38"/>
       <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
+      <c r="I14" s="101"/>
       <c r="J14" s="39"/>
       <c r="K14" s="121"/>
       <c r="L14" s="122"/>
@@ -1928,28 +1933,28 @@
       <c r="T14" s="36"/>
       <c r="U14" s="36"/>
       <c r="V14" s="37"/>
-      <c r="W14" s="171"/>
-      <c r="X14" s="171"/>
-      <c r="Y14" s="171"/>
-      <c r="Z14" s="171"/>
-      <c r="AA14" s="171"/>
-      <c r="AB14" s="171"/>
-      <c r="AC14" s="171"/>
-      <c r="AD14" s="171"/>
-      <c r="AE14" s="171"/>
-      <c r="AF14" s="171"/>
-      <c r="AG14" s="171"/>
-      <c r="AH14" s="171"/>
-      <c r="AI14" s="171"/>
-      <c r="AJ14" s="171"/>
-      <c r="AK14" s="171"/>
-      <c r="AL14" s="171"/>
-    </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A15" s="144" t="s">
+      <c r="W14" s="135"/>
+      <c r="X14" s="135"/>
+      <c r="Y14" s="135"/>
+      <c r="Z14" s="135"/>
+      <c r="AA14" s="135"/>
+      <c r="AB14" s="135"/>
+      <c r="AC14" s="135"/>
+      <c r="AD14" s="135"/>
+      <c r="AE14" s="135"/>
+      <c r="AF14" s="135"/>
+      <c r="AG14" s="135"/>
+      <c r="AH14" s="135"/>
+      <c r="AI14" s="135"/>
+      <c r="AJ14" s="135"/>
+      <c r="AK14" s="135"/>
+      <c r="AL14" s="135"/>
+    </row>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A15" s="170" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="146" t="s">
+      <c r="B15" s="172" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="40"/>
@@ -1972,32 +1977,32 @@
       <c r="T15" s="41"/>
       <c r="U15" s="41"/>
       <c r="V15" s="45"/>
-      <c r="W15" s="171"/>
-      <c r="X15" s="171"/>
-      <c r="Y15" s="171"/>
-      <c r="Z15" s="171"/>
-      <c r="AA15" s="171"/>
-      <c r="AB15" s="171"/>
-      <c r="AC15" s="171"/>
-      <c r="AD15" s="171"/>
-      <c r="AE15" s="171"/>
-      <c r="AF15" s="171"/>
-      <c r="AG15" s="171"/>
-      <c r="AH15" s="171"/>
-      <c r="AI15" s="171"/>
-      <c r="AJ15" s="171"/>
-      <c r="AK15" s="171"/>
-      <c r="AL15" s="171"/>
-    </row>
-    <row r="16" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="145"/>
-      <c r="B16" s="147"/>
+      <c r="W15" s="135"/>
+      <c r="X15" s="135"/>
+      <c r="Y15" s="135"/>
+      <c r="Z15" s="135"/>
+      <c r="AA15" s="135"/>
+      <c r="AB15" s="135"/>
+      <c r="AC15" s="135"/>
+      <c r="AD15" s="135"/>
+      <c r="AE15" s="135"/>
+      <c r="AF15" s="135"/>
+      <c r="AG15" s="135"/>
+      <c r="AH15" s="135"/>
+      <c r="AI15" s="135"/>
+      <c r="AJ15" s="135"/>
+      <c r="AK15" s="135"/>
+      <c r="AL15" s="135"/>
+    </row>
+    <row r="16" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="171"/>
+      <c r="B16" s="173"/>
       <c r="C16" s="46"/>
       <c r="D16" s="47"/>
       <c r="E16" s="47"/>
       <c r="F16" s="50"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="47"/>
+      <c r="G16" s="187"/>
+      <c r="H16" s="101"/>
       <c r="I16" s="47"/>
       <c r="J16" s="49"/>
       <c r="K16" s="46"/>
@@ -2012,26 +2017,26 @@
       <c r="T16" s="47"/>
       <c r="U16" s="47"/>
       <c r="V16" s="50"/>
-      <c r="W16" s="171"/>
-      <c r="X16" s="171"/>
-      <c r="Y16" s="171"/>
-      <c r="Z16" s="171"/>
-      <c r="AA16" s="171"/>
-      <c r="AB16" s="171"/>
-      <c r="AC16" s="171"/>
-      <c r="AD16" s="171"/>
-      <c r="AE16" s="171"/>
-      <c r="AF16" s="171"/>
-      <c r="AG16" s="171"/>
-      <c r="AH16" s="171"/>
-      <c r="AI16" s="171"/>
-      <c r="AJ16" s="171"/>
-      <c r="AK16" s="171"/>
-      <c r="AL16" s="171"/>
-    </row>
-    <row r="17" spans="1:38" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="145"/>
-      <c r="B17" s="148" t="s">
+      <c r="W16" s="135"/>
+      <c r="X16" s="135"/>
+      <c r="Y16" s="135"/>
+      <c r="Z16" s="135"/>
+      <c r="AA16" s="135"/>
+      <c r="AB16" s="135"/>
+      <c r="AC16" s="135"/>
+      <c r="AD16" s="135"/>
+      <c r="AE16" s="135"/>
+      <c r="AF16" s="135"/>
+      <c r="AG16" s="135"/>
+      <c r="AH16" s="135"/>
+      <c r="AI16" s="135"/>
+      <c r="AJ16" s="135"/>
+      <c r="AK16" s="135"/>
+      <c r="AL16" s="135"/>
+    </row>
+    <row r="17" spans="1:38" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="171"/>
+      <c r="B17" s="174" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="51"/>
@@ -2041,8 +2046,8 @@
       <c r="G17" s="55"/>
       <c r="H17" s="52"/>
       <c r="I17" s="52"/>
-      <c r="J17" s="131"/>
-      <c r="K17" s="105"/>
+      <c r="J17" s="54"/>
+      <c r="K17" s="51"/>
       <c r="L17" s="104"/>
       <c r="M17" s="104"/>
       <c r="N17" s="106"/>
@@ -2054,26 +2059,26 @@
       <c r="T17" s="52"/>
       <c r="U17" s="41"/>
       <c r="V17" s="45"/>
-      <c r="W17" s="171"/>
-      <c r="X17" s="171"/>
-      <c r="Y17" s="171"/>
-      <c r="Z17" s="171"/>
-      <c r="AA17" s="171"/>
-      <c r="AB17" s="171"/>
-      <c r="AC17" s="171"/>
-      <c r="AD17" s="171"/>
-      <c r="AE17" s="171"/>
-      <c r="AF17" s="171"/>
-      <c r="AG17" s="171"/>
-      <c r="AH17" s="171"/>
-      <c r="AI17" s="171"/>
-      <c r="AJ17" s="171"/>
-      <c r="AK17" s="171"/>
-      <c r="AL17" s="171"/>
-    </row>
-    <row r="18" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="145"/>
-      <c r="B18" s="149"/>
+      <c r="W17" s="135"/>
+      <c r="X17" s="135"/>
+      <c r="Y17" s="135"/>
+      <c r="Z17" s="135"/>
+      <c r="AA17" s="135"/>
+      <c r="AB17" s="135"/>
+      <c r="AC17" s="135"/>
+      <c r="AD17" s="135"/>
+      <c r="AE17" s="135"/>
+      <c r="AF17" s="135"/>
+      <c r="AG17" s="135"/>
+      <c r="AH17" s="135"/>
+      <c r="AI17" s="135"/>
+      <c r="AJ17" s="135"/>
+      <c r="AK17" s="135"/>
+      <c r="AL17" s="135"/>
+    </row>
+    <row r="18" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="171"/>
+      <c r="B18" s="175"/>
       <c r="C18" s="56"/>
       <c r="D18" s="57"/>
       <c r="E18" s="57"/>
@@ -2083,37 +2088,37 @@
       <c r="I18" s="57"/>
       <c r="J18" s="59"/>
       <c r="K18" s="46"/>
-      <c r="L18" s="47"/>
-      <c r="M18" s="47"/>
-      <c r="N18" s="50"/>
-      <c r="O18" s="60"/>
-      <c r="P18" s="57"/>
+      <c r="L18" s="101"/>
+      <c r="M18" s="101"/>
+      <c r="N18" s="102"/>
+      <c r="O18" s="190"/>
+      <c r="P18" s="191"/>
       <c r="Q18" s="57"/>
       <c r="R18" s="59"/>
-      <c r="S18" s="56"/>
+      <c r="S18" s="193"/>
       <c r="T18" s="57"/>
       <c r="U18" s="57"/>
       <c r="V18" s="58"/>
-      <c r="W18" s="171"/>
-      <c r="X18" s="171"/>
-      <c r="Y18" s="171"/>
-      <c r="Z18" s="171"/>
-      <c r="AA18" s="171"/>
-      <c r="AB18" s="171"/>
-      <c r="AC18" s="171"/>
-      <c r="AD18" s="171"/>
-      <c r="AE18" s="171"/>
-      <c r="AF18" s="171"/>
-      <c r="AG18" s="171"/>
-      <c r="AH18" s="171"/>
-      <c r="AI18" s="171"/>
-      <c r="AJ18" s="171"/>
-      <c r="AK18" s="171"/>
-      <c r="AL18" s="171"/>
-    </row>
-    <row r="19" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="145"/>
-      <c r="B19" s="148" t="s">
+      <c r="W18" s="135"/>
+      <c r="X18" s="135"/>
+      <c r="Y18" s="135"/>
+      <c r="Z18" s="135"/>
+      <c r="AA18" s="135"/>
+      <c r="AB18" s="135"/>
+      <c r="AC18" s="135"/>
+      <c r="AD18" s="135"/>
+      <c r="AE18" s="135"/>
+      <c r="AF18" s="135"/>
+      <c r="AG18" s="135"/>
+      <c r="AH18" s="135"/>
+      <c r="AI18" s="135"/>
+      <c r="AJ18" s="135"/>
+      <c r="AK18" s="135"/>
+      <c r="AL18" s="135"/>
+    </row>
+    <row r="19" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="171"/>
+      <c r="B19" s="174" t="s">
         <v>24</v>
       </c>
       <c r="C19" s="40"/>
@@ -2123,11 +2128,11 @@
       <c r="G19" s="43"/>
       <c r="H19" s="41"/>
       <c r="I19" s="41"/>
-      <c r="J19" s="134"/>
+      <c r="J19" s="133"/>
       <c r="K19" s="105"/>
       <c r="L19" s="104"/>
-      <c r="M19" s="104"/>
-      <c r="N19" s="106"/>
+      <c r="M19" s="52"/>
+      <c r="N19" s="53"/>
       <c r="O19" s="43"/>
       <c r="P19" s="41"/>
       <c r="Q19" s="41"/>
@@ -2136,26 +2141,26 @@
       <c r="T19" s="41"/>
       <c r="U19" s="41"/>
       <c r="V19" s="45"/>
-      <c r="W19" s="171"/>
-      <c r="X19" s="171"/>
-      <c r="Y19" s="171"/>
-      <c r="Z19" s="171"/>
-      <c r="AA19" s="171"/>
-      <c r="AB19" s="171"/>
-      <c r="AC19" s="171"/>
-      <c r="AD19" s="171"/>
-      <c r="AE19" s="171"/>
-      <c r="AF19" s="171"/>
-      <c r="AG19" s="171"/>
-      <c r="AH19" s="171"/>
-      <c r="AI19" s="171"/>
-      <c r="AJ19" s="171"/>
-      <c r="AK19" s="171"/>
-      <c r="AL19" s="171"/>
-    </row>
-    <row r="20" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="145"/>
-      <c r="B20" s="149"/>
+      <c r="W19" s="135"/>
+      <c r="X19" s="135"/>
+      <c r="Y19" s="135"/>
+      <c r="Z19" s="135"/>
+      <c r="AA19" s="135"/>
+      <c r="AB19" s="135"/>
+      <c r="AC19" s="135"/>
+      <c r="AD19" s="135"/>
+      <c r="AE19" s="135"/>
+      <c r="AF19" s="135"/>
+      <c r="AG19" s="135"/>
+      <c r="AH19" s="135"/>
+      <c r="AI19" s="135"/>
+      <c r="AJ19" s="135"/>
+      <c r="AK19" s="135"/>
+      <c r="AL19" s="135"/>
+    </row>
+    <row r="20" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="171"/>
+      <c r="B20" s="175"/>
       <c r="C20" s="46"/>
       <c r="D20" s="47"/>
       <c r="E20" s="47"/>
@@ -2163,8 +2168,8 @@
       <c r="G20" s="48"/>
       <c r="H20" s="47"/>
       <c r="I20" s="47"/>
-      <c r="J20" s="49"/>
-      <c r="K20" s="46"/>
+      <c r="J20" s="189"/>
+      <c r="K20" s="188"/>
       <c r="L20" s="47"/>
       <c r="M20" s="47"/>
       <c r="N20" s="50"/>
@@ -2176,26 +2181,26 @@
       <c r="T20" s="47"/>
       <c r="U20" s="47"/>
       <c r="V20" s="50"/>
-      <c r="W20" s="171"/>
-      <c r="X20" s="171"/>
-      <c r="Y20" s="171"/>
-      <c r="Z20" s="171"/>
-      <c r="AA20" s="171"/>
-      <c r="AB20" s="171"/>
-      <c r="AC20" s="171"/>
-      <c r="AD20" s="171"/>
-      <c r="AE20" s="171"/>
-      <c r="AF20" s="171"/>
-      <c r="AG20" s="171"/>
-      <c r="AH20" s="171"/>
-      <c r="AI20" s="171"/>
-      <c r="AJ20" s="171"/>
-      <c r="AK20" s="171"/>
-      <c r="AL20" s="171"/>
-    </row>
-    <row r="21" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="145"/>
-      <c r="B21" s="148" t="s">
+      <c r="W20" s="135"/>
+      <c r="X20" s="135"/>
+      <c r="Y20" s="135"/>
+      <c r="Z20" s="135"/>
+      <c r="AA20" s="135"/>
+      <c r="AB20" s="135"/>
+      <c r="AC20" s="135"/>
+      <c r="AD20" s="135"/>
+      <c r="AE20" s="135"/>
+      <c r="AF20" s="135"/>
+      <c r="AG20" s="135"/>
+      <c r="AH20" s="135"/>
+      <c r="AI20" s="135"/>
+      <c r="AJ20" s="135"/>
+      <c r="AK20" s="135"/>
+      <c r="AL20" s="135"/>
+    </row>
+    <row r="21" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="171"/>
+      <c r="B21" s="174" t="s">
         <v>25</v>
       </c>
       <c r="C21" s="40"/>
@@ -2207,9 +2212,9 @@
       <c r="I21" s="41"/>
       <c r="J21" s="42"/>
       <c r="K21" s="68"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="42"/>
+      <c r="L21" s="41"/>
+      <c r="M21" s="41"/>
+      <c r="N21" s="45"/>
       <c r="O21" s="55"/>
       <c r="P21" s="52"/>
       <c r="Q21" s="52"/>
@@ -2218,26 +2223,26 @@
       <c r="T21" s="52"/>
       <c r="U21" s="52"/>
       <c r="V21" s="53"/>
-      <c r="W21" s="171"/>
-      <c r="X21" s="171"/>
-      <c r="Y21" s="171"/>
-      <c r="Z21" s="171"/>
-      <c r="AA21" s="171"/>
-      <c r="AB21" s="171"/>
-      <c r="AC21" s="171"/>
-      <c r="AD21" s="171"/>
-      <c r="AE21" s="171"/>
-      <c r="AF21" s="171"/>
-      <c r="AG21" s="171"/>
-      <c r="AH21" s="171"/>
-      <c r="AI21" s="171"/>
-      <c r="AJ21" s="171"/>
-      <c r="AK21" s="171"/>
-      <c r="AL21" s="171"/>
-    </row>
-    <row r="22" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="145"/>
-      <c r="B22" s="149"/>
+      <c r="W21" s="135"/>
+      <c r="X21" s="135"/>
+      <c r="Y21" s="135"/>
+      <c r="Z21" s="135"/>
+      <c r="AA21" s="135"/>
+      <c r="AB21" s="135"/>
+      <c r="AC21" s="135"/>
+      <c r="AD21" s="135"/>
+      <c r="AE21" s="135"/>
+      <c r="AF21" s="135"/>
+      <c r="AG21" s="135"/>
+      <c r="AH21" s="135"/>
+      <c r="AI21" s="135"/>
+      <c r="AJ21" s="135"/>
+      <c r="AK21" s="135"/>
+      <c r="AL21" s="135"/>
+    </row>
+    <row r="22" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="171"/>
+      <c r="B22" s="175"/>
       <c r="C22" s="46"/>
       <c r="D22" s="47"/>
       <c r="E22" s="47"/>
@@ -2245,8 +2250,8 @@
       <c r="G22" s="46"/>
       <c r="H22" s="47"/>
       <c r="I22" s="47"/>
-      <c r="J22" s="50"/>
-      <c r="K22" s="46"/>
+      <c r="J22" s="102"/>
+      <c r="K22" s="188"/>
       <c r="L22" s="47"/>
       <c r="M22" s="47"/>
       <c r="N22" s="50"/>
@@ -2258,26 +2263,26 @@
       <c r="T22" s="57"/>
       <c r="U22" s="57"/>
       <c r="V22" s="58"/>
-      <c r="W22" s="171"/>
-      <c r="X22" s="171"/>
-      <c r="Y22" s="171"/>
-      <c r="Z22" s="171"/>
-      <c r="AA22" s="171"/>
-      <c r="AB22" s="171"/>
-      <c r="AC22" s="171"/>
-      <c r="AD22" s="171"/>
-      <c r="AE22" s="171"/>
-      <c r="AF22" s="171"/>
-      <c r="AG22" s="171"/>
-      <c r="AH22" s="171"/>
-      <c r="AI22" s="171"/>
-      <c r="AJ22" s="171"/>
-      <c r="AK22" s="171"/>
-      <c r="AL22" s="171"/>
-    </row>
-    <row r="23" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="145"/>
-      <c r="B23" s="146" t="s">
+      <c r="W22" s="135"/>
+      <c r="X22" s="135"/>
+      <c r="Y22" s="135"/>
+      <c r="Z22" s="135"/>
+      <c r="AA22" s="135"/>
+      <c r="AB22" s="135"/>
+      <c r="AC22" s="135"/>
+      <c r="AD22" s="135"/>
+      <c r="AE22" s="135"/>
+      <c r="AF22" s="135"/>
+      <c r="AG22" s="135"/>
+      <c r="AH22" s="135"/>
+      <c r="AI22" s="135"/>
+      <c r="AJ22" s="135"/>
+      <c r="AK22" s="135"/>
+      <c r="AL22" s="135"/>
+    </row>
+    <row r="23" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="171"/>
+      <c r="B23" s="172" t="s">
         <v>26</v>
       </c>
       <c r="C23" s="40"/>
@@ -2287,8 +2292,8 @@
       <c r="G23" s="40"/>
       <c r="H23" s="41"/>
       <c r="I23" s="41"/>
-      <c r="J23" s="42"/>
-      <c r="K23" s="68"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="40"/>
       <c r="L23" s="7"/>
       <c r="M23" s="7"/>
       <c r="N23" s="42"/>
@@ -2300,26 +2305,26 @@
       <c r="T23" s="41"/>
       <c r="U23" s="41"/>
       <c r="V23" s="45"/>
-      <c r="W23" s="171"/>
-      <c r="X23" s="171"/>
-      <c r="Y23" s="171"/>
-      <c r="Z23" s="171"/>
-      <c r="AA23" s="171"/>
-      <c r="AB23" s="171"/>
-      <c r="AC23" s="171"/>
-      <c r="AD23" s="171"/>
-      <c r="AE23" s="171"/>
-      <c r="AF23" s="171"/>
-      <c r="AG23" s="171"/>
-      <c r="AH23" s="171"/>
-      <c r="AI23" s="171"/>
-      <c r="AJ23" s="171"/>
-      <c r="AK23" s="171"/>
-      <c r="AL23" s="171"/>
-    </row>
-    <row r="24" spans="1:38" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="145"/>
-      <c r="B24" s="147"/>
+      <c r="W23" s="135"/>
+      <c r="X23" s="135"/>
+      <c r="Y23" s="135"/>
+      <c r="Z23" s="135"/>
+      <c r="AA23" s="135"/>
+      <c r="AB23" s="135"/>
+      <c r="AC23" s="135"/>
+      <c r="AD23" s="135"/>
+      <c r="AE23" s="135"/>
+      <c r="AF23" s="135"/>
+      <c r="AG23" s="135"/>
+      <c r="AH23" s="135"/>
+      <c r="AI23" s="135"/>
+      <c r="AJ23" s="135"/>
+      <c r="AK23" s="135"/>
+      <c r="AL23" s="135"/>
+    </row>
+    <row r="24" spans="1:38" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="171"/>
+      <c r="B24" s="173"/>
       <c r="C24" s="46"/>
       <c r="D24" s="47"/>
       <c r="E24" s="47"/>
@@ -2329,39 +2334,39 @@
       <c r="I24" s="47"/>
       <c r="J24" s="50"/>
       <c r="K24" s="46"/>
-      <c r="L24" s="47"/>
-      <c r="M24" s="47"/>
-      <c r="N24" s="50"/>
-      <c r="O24" s="46"/>
-      <c r="P24" s="47"/>
+      <c r="L24" s="101"/>
+      <c r="M24" s="101"/>
+      <c r="N24" s="102"/>
+      <c r="O24" s="188"/>
+      <c r="P24" s="101"/>
       <c r="Q24" s="47"/>
       <c r="R24" s="50"/>
-      <c r="S24" s="46"/>
+      <c r="S24" s="188"/>
       <c r="T24" s="47"/>
       <c r="U24" s="47"/>
       <c r="V24" s="50"/>
-      <c r="W24" s="171"/>
-      <c r="X24" s="171"/>
-      <c r="Y24" s="171"/>
-      <c r="Z24" s="171"/>
-      <c r="AA24" s="171"/>
-      <c r="AB24" s="171"/>
-      <c r="AC24" s="171"/>
-      <c r="AD24" s="171"/>
-      <c r="AE24" s="171"/>
-      <c r="AF24" s="171"/>
-      <c r="AG24" s="171"/>
-      <c r="AH24" s="171"/>
-      <c r="AI24" s="171"/>
-      <c r="AJ24" s="171"/>
-      <c r="AK24" s="171"/>
-      <c r="AL24" s="171"/>
-    </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A25" s="150" t="s">
+      <c r="W24" s="135"/>
+      <c r="X24" s="135"/>
+      <c r="Y24" s="135"/>
+      <c r="Z24" s="135"/>
+      <c r="AA24" s="135"/>
+      <c r="AB24" s="135"/>
+      <c r="AC24" s="135"/>
+      <c r="AD24" s="135"/>
+      <c r="AE24" s="135"/>
+      <c r="AF24" s="135"/>
+      <c r="AG24" s="135"/>
+      <c r="AH24" s="135"/>
+      <c r="AI24" s="135"/>
+      <c r="AJ24" s="135"/>
+      <c r="AK24" s="135"/>
+      <c r="AL24" s="135"/>
+    </row>
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A25" s="145" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="153" t="s">
+      <c r="B25" s="148" t="s">
         <v>29</v>
       </c>
       <c r="C25" s="126"/>
@@ -2376,34 +2381,34 @@
       <c r="L25" s="127"/>
       <c r="M25" s="127"/>
       <c r="N25" s="128"/>
-      <c r="O25" s="185"/>
+      <c r="O25" s="141"/>
       <c r="P25" s="29"/>
       <c r="Q25" s="29"/>
-      <c r="R25" s="186"/>
+      <c r="R25" s="142"/>
       <c r="S25" s="126"/>
       <c r="T25" s="127"/>
       <c r="U25" s="127"/>
       <c r="V25" s="128"/>
-      <c r="W25" s="171"/>
-      <c r="X25" s="171"/>
-      <c r="Y25" s="171"/>
-      <c r="Z25" s="171"/>
-      <c r="AA25" s="171"/>
-      <c r="AB25" s="171"/>
-      <c r="AC25" s="171"/>
-      <c r="AD25" s="171"/>
-      <c r="AE25" s="171"/>
-      <c r="AF25" s="171"/>
-      <c r="AG25" s="171"/>
-      <c r="AH25" s="171"/>
-      <c r="AI25" s="171"/>
-      <c r="AJ25" s="171"/>
-      <c r="AK25" s="171"/>
-      <c r="AL25" s="171"/>
-    </row>
-    <row r="26" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="151"/>
-      <c r="B26" s="154"/>
+      <c r="W25" s="135"/>
+      <c r="X25" s="135"/>
+      <c r="Y25" s="135"/>
+      <c r="Z25" s="135"/>
+      <c r="AA25" s="135"/>
+      <c r="AB25" s="135"/>
+      <c r="AC25" s="135"/>
+      <c r="AD25" s="135"/>
+      <c r="AE25" s="135"/>
+      <c r="AF25" s="135"/>
+      <c r="AG25" s="135"/>
+      <c r="AH25" s="135"/>
+      <c r="AI25" s="135"/>
+      <c r="AJ25" s="135"/>
+      <c r="AK25" s="135"/>
+      <c r="AL25" s="135"/>
+    </row>
+    <row r="26" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="146"/>
+      <c r="B26" s="149"/>
       <c r="C26" s="111"/>
       <c r="D26" s="112"/>
       <c r="E26" s="112"/>
@@ -2418,32 +2423,32 @@
       <c r="N26" s="113"/>
       <c r="O26" s="114"/>
       <c r="P26" s="112"/>
-      <c r="Q26" s="112"/>
-      <c r="R26" s="115"/>
+      <c r="Q26" s="191"/>
+      <c r="R26" s="192"/>
       <c r="S26" s="111"/>
       <c r="T26" s="112"/>
       <c r="U26" s="112"/>
       <c r="V26" s="113"/>
-      <c r="W26" s="171"/>
-      <c r="X26" s="171"/>
-      <c r="Y26" s="171"/>
-      <c r="Z26" s="171"/>
-      <c r="AA26" s="171"/>
-      <c r="AB26" s="171"/>
-      <c r="AC26" s="171"/>
-      <c r="AD26" s="171"/>
-      <c r="AE26" s="171"/>
-      <c r="AF26" s="171"/>
-      <c r="AG26" s="171"/>
-      <c r="AH26" s="171"/>
-      <c r="AI26" s="171"/>
-      <c r="AJ26" s="171"/>
-      <c r="AK26" s="171"/>
-      <c r="AL26" s="171"/>
-    </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A27" s="151"/>
-      <c r="B27" s="153" t="s">
+      <c r="W26" s="135"/>
+      <c r="X26" s="135"/>
+      <c r="Y26" s="135"/>
+      <c r="Z26" s="135"/>
+      <c r="AA26" s="135"/>
+      <c r="AB26" s="135"/>
+      <c r="AC26" s="135"/>
+      <c r="AD26" s="135"/>
+      <c r="AE26" s="135"/>
+      <c r="AF26" s="135"/>
+      <c r="AG26" s="135"/>
+      <c r="AH26" s="135"/>
+      <c r="AI26" s="135"/>
+      <c r="AJ26" s="135"/>
+      <c r="AK26" s="135"/>
+      <c r="AL26" s="135"/>
+    </row>
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A27" s="146"/>
+      <c r="B27" s="148" t="s">
         <v>28</v>
       </c>
       <c r="C27" s="108"/>
@@ -2458,34 +2463,34 @@
       <c r="L27" s="61"/>
       <c r="M27" s="61"/>
       <c r="N27" s="109"/>
-      <c r="O27" s="133"/>
-      <c r="P27" s="132"/>
-      <c r="Q27" s="132"/>
-      <c r="R27" s="134"/>
+      <c r="O27" s="132"/>
+      <c r="P27" s="131"/>
+      <c r="Q27" s="131"/>
+      <c r="R27" s="133"/>
       <c r="S27" s="108"/>
       <c r="T27" s="61"/>
       <c r="U27" s="61"/>
       <c r="V27" s="109"/>
-      <c r="W27" s="171"/>
-      <c r="X27" s="171"/>
-      <c r="Y27" s="171"/>
-      <c r="Z27" s="171"/>
-      <c r="AA27" s="171"/>
-      <c r="AB27" s="171"/>
-      <c r="AC27" s="171"/>
-      <c r="AD27" s="171"/>
-      <c r="AE27" s="171"/>
-      <c r="AF27" s="171"/>
-      <c r="AG27" s="171"/>
-      <c r="AH27" s="171"/>
-      <c r="AI27" s="171"/>
-      <c r="AJ27" s="171"/>
-      <c r="AK27" s="171"/>
-      <c r="AL27" s="171"/>
-    </row>
-    <row r="28" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="152"/>
-      <c r="B28" s="154"/>
+      <c r="W27" s="135"/>
+      <c r="X27" s="135"/>
+      <c r="Y27" s="135"/>
+      <c r="Z27" s="135"/>
+      <c r="AA27" s="135"/>
+      <c r="AB27" s="135"/>
+      <c r="AC27" s="135"/>
+      <c r="AD27" s="135"/>
+      <c r="AE27" s="135"/>
+      <c r="AF27" s="135"/>
+      <c r="AG27" s="135"/>
+      <c r="AH27" s="135"/>
+      <c r="AI27" s="135"/>
+      <c r="AJ27" s="135"/>
+      <c r="AK27" s="135"/>
+      <c r="AL27" s="135"/>
+    </row>
+    <row r="28" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="147"/>
+      <c r="B28" s="149"/>
       <c r="C28" s="116"/>
       <c r="D28" s="117"/>
       <c r="E28" s="117"/>
@@ -2500,34 +2505,34 @@
       <c r="N28" s="118"/>
       <c r="O28" s="119"/>
       <c r="P28" s="117"/>
-      <c r="Q28" s="117"/>
-      <c r="R28" s="120"/>
+      <c r="Q28" s="101"/>
+      <c r="R28" s="189"/>
       <c r="S28" s="116"/>
       <c r="T28" s="117"/>
       <c r="U28" s="117"/>
       <c r="V28" s="118"/>
-      <c r="W28" s="171"/>
-      <c r="X28" s="171"/>
-      <c r="Y28" s="171"/>
-      <c r="Z28" s="171"/>
-      <c r="AA28" s="171"/>
-      <c r="AB28" s="171"/>
-      <c r="AC28" s="171"/>
-      <c r="AD28" s="171"/>
-      <c r="AE28" s="171"/>
-      <c r="AF28" s="171"/>
-      <c r="AG28" s="171"/>
-      <c r="AH28" s="171"/>
-      <c r="AI28" s="171"/>
-      <c r="AJ28" s="171"/>
-      <c r="AK28" s="171"/>
-      <c r="AL28" s="171"/>
-    </row>
-    <row r="29" spans="1:38" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="141" t="s">
+      <c r="W28" s="135"/>
+      <c r="X28" s="135"/>
+      <c r="Y28" s="135"/>
+      <c r="Z28" s="135"/>
+      <c r="AA28" s="135"/>
+      <c r="AB28" s="135"/>
+      <c r="AC28" s="135"/>
+      <c r="AD28" s="135"/>
+      <c r="AE28" s="135"/>
+      <c r="AF28" s="135"/>
+      <c r="AG28" s="135"/>
+      <c r="AH28" s="135"/>
+      <c r="AI28" s="135"/>
+      <c r="AJ28" s="135"/>
+      <c r="AK28" s="135"/>
+      <c r="AL28" s="135"/>
+    </row>
+    <row r="29" spans="1:38" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="176" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="142" t="s">
+      <c r="B29" s="168" t="s">
         <v>8</v>
       </c>
       <c r="C29" s="63"/>
@@ -2550,26 +2555,26 @@
       <c r="T29" s="96"/>
       <c r="U29" s="96"/>
       <c r="V29" s="97"/>
-      <c r="W29" s="171"/>
-      <c r="X29" s="171"/>
-      <c r="Y29" s="171"/>
-      <c r="Z29" s="171"/>
-      <c r="AA29" s="171"/>
-      <c r="AB29" s="171"/>
-      <c r="AC29" s="171"/>
-      <c r="AD29" s="171"/>
-      <c r="AE29" s="171"/>
-      <c r="AF29" s="171"/>
-      <c r="AG29" s="171"/>
-      <c r="AH29" s="171"/>
-      <c r="AI29" s="171"/>
-      <c r="AJ29" s="171"/>
-      <c r="AK29" s="171"/>
-      <c r="AL29" s="171"/>
-    </row>
-    <row r="30" spans="1:38" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="174"/>
-      <c r="B30" s="143"/>
+      <c r="W29" s="135"/>
+      <c r="X29" s="135"/>
+      <c r="Y29" s="135"/>
+      <c r="Z29" s="135"/>
+      <c r="AA29" s="135"/>
+      <c r="AB29" s="135"/>
+      <c r="AC29" s="135"/>
+      <c r="AD29" s="135"/>
+      <c r="AE29" s="135"/>
+      <c r="AF29" s="135"/>
+      <c r="AG29" s="135"/>
+      <c r="AH29" s="135"/>
+      <c r="AI29" s="135"/>
+      <c r="AJ29" s="135"/>
+      <c r="AK29" s="135"/>
+      <c r="AL29" s="135"/>
+    </row>
+    <row r="30" spans="1:38" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="177"/>
+      <c r="B30" s="169"/>
       <c r="C30" s="69"/>
       <c r="D30" s="70"/>
       <c r="E30" s="70"/>
@@ -2587,64 +2592,85 @@
       <c r="Q30" s="70"/>
       <c r="R30" s="73"/>
       <c r="S30" s="69"/>
-      <c r="T30" s="70"/>
-      <c r="U30" s="70"/>
-      <c r="V30" s="71"/>
-      <c r="W30" s="171"/>
-      <c r="X30" s="171"/>
-      <c r="Y30" s="171"/>
-      <c r="Z30" s="171"/>
-      <c r="AA30" s="171"/>
-      <c r="AB30" s="171"/>
-      <c r="AC30" s="171"/>
-      <c r="AD30" s="171"/>
-      <c r="AE30" s="171"/>
-      <c r="AF30" s="171"/>
-      <c r="AG30" s="171"/>
-      <c r="AH30" s="171"/>
-      <c r="AI30" s="171"/>
-      <c r="AJ30" s="171"/>
-      <c r="AK30" s="171"/>
-      <c r="AL30" s="171"/>
-    </row>
-    <row r="31" spans="1:38" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="171"/>
-      <c r="B31" s="171"/>
-      <c r="C31" s="171"/>
-      <c r="D31" s="171"/>
-      <c r="E31" s="171"/>
-      <c r="F31" s="171"/>
-      <c r="G31" s="171"/>
-      <c r="H31" s="171"/>
-      <c r="I31" s="171"/>
-      <c r="J31" s="171"/>
-      <c r="K31" s="171"/>
-      <c r="L31" s="171"/>
-      <c r="M31" s="171"/>
-      <c r="N31" s="171"/>
-      <c r="O31" s="171"/>
-      <c r="P31" s="171"/>
-    </row>
-    <row r="32" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="171"/>
-      <c r="B32" s="171"/>
-      <c r="C32" s="171"/>
-      <c r="D32" s="171"/>
-      <c r="E32" s="171"/>
-      <c r="F32" s="171"/>
-      <c r="G32" s="171"/>
-      <c r="H32" s="171"/>
-      <c r="I32" s="171"/>
-      <c r="J32" s="171"/>
-      <c r="K32" s="171"/>
-      <c r="L32" s="171"/>
-      <c r="M32" s="171"/>
-      <c r="N32" s="171"/>
-      <c r="O32" s="171"/>
-      <c r="P32" s="171"/>
+      <c r="T30" s="101"/>
+      <c r="U30" s="101"/>
+      <c r="V30" s="102"/>
+      <c r="W30" s="135"/>
+      <c r="X30" s="135"/>
+      <c r="Y30" s="135"/>
+      <c r="Z30" s="135"/>
+      <c r="AA30" s="135"/>
+      <c r="AB30" s="135"/>
+      <c r="AC30" s="135"/>
+      <c r="AD30" s="135"/>
+      <c r="AE30" s="135"/>
+      <c r="AF30" s="135"/>
+      <c r="AG30" s="135"/>
+      <c r="AH30" s="135"/>
+      <c r="AI30" s="135"/>
+      <c r="AJ30" s="135"/>
+      <c r="AK30" s="135"/>
+      <c r="AL30" s="135"/>
+    </row>
+    <row r="31" spans="1:38" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="135"/>
+      <c r="B31" s="135"/>
+      <c r="C31" s="135"/>
+      <c r="D31" s="135"/>
+      <c r="E31" s="135"/>
+      <c r="F31" s="135"/>
+      <c r="G31" s="135"/>
+      <c r="H31" s="135"/>
+      <c r="I31" s="135"/>
+      <c r="J31" s="135"/>
+      <c r="K31" s="135"/>
+      <c r="L31" s="135"/>
+      <c r="M31" s="135"/>
+      <c r="N31" s="135"/>
+      <c r="O31" s="135"/>
+      <c r="P31" s="135"/>
+    </row>
+    <row r="32" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="135"/>
+      <c r="B32" s="135"/>
+      <c r="C32" s="135"/>
+      <c r="D32" s="135"/>
+      <c r="E32" s="135"/>
+      <c r="F32" s="135"/>
+      <c r="G32" s="135"/>
+      <c r="H32" s="135"/>
+      <c r="I32" s="135"/>
+      <c r="J32" s="135"/>
+      <c r="K32" s="135"/>
+      <c r="L32" s="135"/>
+      <c r="M32" s="135"/>
+      <c r="N32" s="135"/>
+      <c r="O32" s="135"/>
+      <c r="P32" s="135"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="W5:Z5"/>
+    <mergeCell ref="AA5:AD5"/>
+    <mergeCell ref="AE5:AH5"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="O5:R5"/>
+    <mergeCell ref="S5:V5"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="O6:R6"/>
+    <mergeCell ref="S6:V6"/>
+    <mergeCell ref="A1:F4"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="A29:A30"/>
     <mergeCell ref="AI5:AL5"/>
     <mergeCell ref="AI6:AL6"/>
     <mergeCell ref="A25:A28"/>
@@ -2661,27 +2687,6 @@
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C6:F6"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="A15:A24"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="O6:R6"/>
-    <mergeCell ref="S6:V6"/>
-    <mergeCell ref="A1:F4"/>
-    <mergeCell ref="W5:Z5"/>
-    <mergeCell ref="AA5:AD5"/>
-    <mergeCell ref="AE5:AH5"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="O5:R5"/>
-    <mergeCell ref="S5:V5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>